<commit_message>
finalized Evaluator class with retriever evaluation
</commit_message>
<xml_diff>
--- a/backend/evaluation/FAQ.xlsx
+++ b/backend/evaluation/FAQ.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danam\Git\semester_6\LAB\FinalProject\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danam\Git\semester_6\LAB\FinalProject\backend\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822AA4E2-37DE-42BF-A0D6-25C00D93AFB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4EE760-2852-48BA-81E3-0DA3E975836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{16688047-19B4-47FE-ADAF-402B6B8A82DD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Who is eligible to transportation for treatments and examinations for dialysis patients up to 18 years of age?</t>
   </si>
@@ -116,13 +116,49 @@
   </si>
   <si>
     <t>answer</t>
+  </si>
+  <si>
+    <t>relevant_chunks_id</t>
+  </si>
+  <si>
+    <t>id1,id2,id3</t>
+  </si>
+  <si>
+    <t>id1,id2,id4</t>
+  </si>
+  <si>
+    <t>id1,id2,id5</t>
+  </si>
+  <si>
+    <t>id1,id2,id6</t>
+  </si>
+  <si>
+    <t>id1,id2,id7</t>
+  </si>
+  <si>
+    <t>id1,id2,id8</t>
+  </si>
+  <si>
+    <t>id1,id2,id9</t>
+  </si>
+  <si>
+    <t>id1,id2,id10</t>
+  </si>
+  <si>
+    <t>id1,id2,id11</t>
+  </si>
+  <si>
+    <t>id1,id2,id12</t>
+  </si>
+  <si>
+    <t>id1,id2,id13</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +175,12 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -164,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -190,6 +232,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -525,7 +570,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80926113-D334-437D-8812-60542D85F9A4}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
@@ -534,163 +579,205 @@
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="206.81640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" customWidth="1"/>
-    <col min="5" max="5" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="206.81640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="5.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>87</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>32</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>10</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>34</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>176</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>122</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>229</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>192</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>137</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>171</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="7">
         <v>161</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D12" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="1"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added support to configurate different evaluation aspects
</commit_message>
<xml_diff>
--- a/backend/evaluation/FAQ.xlsx
+++ b/backend/evaluation/FAQ.xlsx
@@ -8,13 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danam\Git\semester_6\LAB\FinalProject\backend\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4EE760-2852-48BA-81E3-0DA3E975836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720536BD-07AB-4A2F-BE13-02049E538F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{16688047-19B4-47FE-ADAF-402B6B8A82DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="IDS" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IDS!$A$60:$B$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$11</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>Who is eligible to transportation for treatments and examinations for dialysis patients up to 18 years of age?</t>
   </si>
@@ -84,19 +89,6 @@
     <t>My Maccabi, gold and silver companies interested in examination without medical need - in Asuta salons only.</t>
   </si>
   <si>
-    <t>What is the entitlement for wrist sheild?</t>
-  </si>
-  <si>
-    <t>Only one accessory per limb (for example, one per hand), once a calendar year with agreed suppliers.Seniority is required in the insurance plan
-The service is given to Maccabi Shelli and Maccabi Gold members after 12 months from the date of joining the program.</t>
-  </si>
-  <si>
-    <t>Is there a treatment of eating disorders in Holon?</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>What is a “home visit”?</t>
   </si>
   <si>
@@ -121,44 +113,257 @@
     <t>relevant_chunks_id</t>
   </si>
   <si>
-    <t>id1,id2,id3</t>
-  </si>
-  <si>
-    <t>id1,id2,id4</t>
-  </si>
-  <si>
-    <t>id1,id2,id5</t>
-  </si>
-  <si>
-    <t>id1,id2,id6</t>
-  </si>
-  <si>
-    <t>id1,id2,id7</t>
-  </si>
-  <si>
-    <t>id1,id2,id8</t>
-  </si>
-  <si>
-    <t>id1,id2,id9</t>
-  </si>
-  <si>
-    <t>id1,id2,id10</t>
-  </si>
-  <si>
-    <t>id1,id2,id11</t>
-  </si>
-  <si>
-    <t>id1,id2,id12</t>
-  </si>
-  <si>
-    <t>id1,id2,id13</t>
+    <t>6714d62959be40a379e53a30</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2f</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2e</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2d</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2c</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2b</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2a</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a29</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a28</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a27</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a26</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a25</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a20</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a21</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a22</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a23</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a24</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1b</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1f</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1e</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1d</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1c</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a16</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1a</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a17</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a18</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a19</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f4</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f9</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f5</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f6</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f7</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f8</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539fa</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539fb</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539fc</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539fd</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539fe</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539ff</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a00</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a01</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a02</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a03</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a04</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a05</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a06</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a07</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a08</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a09</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0a</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a10</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a11</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a12</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a13</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a14</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a15</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0b</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0c</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0d</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0e</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a0f</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f3</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f2</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f1</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f0</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539ef</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f4,6714d62959be40a379e539f5,6714d62959be40a379e539f6,6714d62959be40a379e539f7,6714d62959be40a379e539f8,6714d62959be40a379e539f9,6714d62959be40a379e539fa,6714d62959be40a379e539fb,6714d62959be40a379e539fc,6714d62959be40a379e539fd,6714d62959be40a379e539fe,6714d62959be40a379e539ff,6714d62959be40a379e53a00,6714d62959be40a379e53a01,6714d62959be40a379e53a02,6714d62959be40a379e53a03,6714d62959be40a379e53a04,6714d62959be40a379e53a05,6714d62959be40a379e53a06,6714d62959be40a379e53a07,6714d62959be40a379e53a08,6714d62959be40a379e53a09,6714d62959be40a379e53a0a,6714d62959be40a379e53a0b,6714d62959be40a379e53a0c,6714d62959be40a379e53a0d,6714d62959be40a379e53a0e,6714d62959be40a379e53a0f,6714d62959be40a379e53a10,6714d62959be40a379e53a11,6714d62959be40a379e53a12,6714d62959be40a379e53a13,6714d62959be40a379e53a14,6714d62959be40a379e53a15</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a16,6714d62959be40a379e53a17,6714d62959be40a379e53a18,6714d62959be40a379e53a19,6714d62959be40a379e53a1a</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1b,6714d62959be40a379e53a1c</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a1d,6714d62959be40a379e53a1e,6714d62959be40a379e53a1f</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a20,6714d62959be40a379e53a21,6714d62959be40a379e53a22,6714d62959be40a379e53a23,6714d62959be40a379e53a24</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a25,6714d62959be40a379e53a26,6714d62959be40a379e53a276714d62959be40a379e53a28</t>
+  </si>
+  <si>
+    <r>
+      <t>6714d62959be40a379e53a29,6714d62959be40a379e53a2a,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7"/>
+        <color rgb="FFD83713"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>6714d62959be40a379e53a2b,6714d62959be40a379e53a2c</t>
+    </r>
+  </si>
+  <si>
+    <t>6714d62959be40a379e53a2d,6714d62959be40a379e53a2e,6714d62959be40a379e53a2f,6714d62959be40a379e53a30</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539ef,6714d62959be40a379e539f0,6714d62959be40a379e539f1</t>
+  </si>
+  <si>
+    <t>6714d62959be40a379e539f2,6714d62959be40a379e539f3</t>
+  </si>
+  <si>
+    <t>There is no clinic for treatment of eating disorders in Holon</t>
+  </si>
+  <si>
+    <t>Is there aclinic for treatment of eating disorders in Holon?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,6 +390,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFD83713"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7"/>
+      <color rgb="FFD83713"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -206,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -233,8 +451,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -570,57 +789,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80926113-D334-437D-8812-60542D85F9A4}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.36328125" customWidth="1"/>
+    <col min="2" max="2" width="42.08984375" customWidth="1"/>
     <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="206.81640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="5.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
-        <v>87</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="B2" s="11" t="str">
+        <f>VLOOKUP($A2,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e539ef,6714d62959be40a379e539f0,6714d62959be40a379e539f1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>32</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>27</v>
+      <c r="B3" s="11" t="str">
+        <f>VLOOKUP($A3,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a16,6714d62959be40a379e53a17,6714d62959be40a379e53a18,6714d62959be40a379e53a19,6714d62959be40a379e53a1a</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>1</v>
@@ -629,82 +850,88 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
-        <v>10</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="B4" s="11" t="str">
+        <f>VLOOKUP($A4,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a1b,6714d62959be40a379e53a1c</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
-        <v>34</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>29</v>
+        <v>87</v>
+      </c>
+      <c r="B5" s="11" t="str">
+        <f>VLOOKUP($A5,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a20,6714d62959be40a379e53a21,6714d62959be40a379e53a22,6714d62959be40a379e53a23,6714d62959be40a379e53a24</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
-        <v>176</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>30</v>
+        <v>122</v>
+      </c>
+      <c r="B6" s="11" t="str">
+        <f>VLOOKUP($A6,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e539f2,6714d62959be40a379e539f3</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="304.5" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
-        <v>122</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>31</v>
+        <v>137</v>
+      </c>
+      <c r="B7" s="11" t="str">
+        <f>VLOOKUP($A7,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e539f4,6714d62959be40a379e539f5,6714d62959be40a379e539f6,6714d62959be40a379e539f7,6714d62959be40a379e539f8,6714d62959be40a379e539f9,6714d62959be40a379e539fa,6714d62959be40a379e539fb,6714d62959be40a379e539fc,6714d62959be40a379e539fd,6714d62959be40a379e539fe,6714d62959be40a379e539ff,6714d62959be40a379e53a00,6714d62959be40a379e53a01,6714d62959be40a379e53a02,6714d62959be40a379e53a03,6714d62959be40a379e53a04,6714d62959be40a379e53a05,6714d62959be40a379e53a06,6714d62959be40a379e53a07,6714d62959be40a379e53a08,6714d62959be40a379e53a09,6714d62959be40a379e53a0a,6714d62959be40a379e53a0b,6714d62959be40a379e53a0c,6714d62959be40a379e53a0d,6714d62959be40a379e53a0e,6714d62959be40a379e53a0f,6714d62959be40a379e53a10,6714d62959be40a379e53a11,6714d62959be40a379e53a12,6714d62959be40a379e53a13,6714d62959be40a379e53a14,6714d62959be40a379e53a15</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
-        <v>229</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>12</v>
+        <v>161</v>
+      </c>
+      <c r="B8" s="11" t="str">
+        <f>VLOOKUP($A8,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a2d,6714d62959be40a379e53a2e,6714d62959be40a379e53a2f,6714d62959be40a379e53a30</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
-        <v>192</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>33</v>
+        <v>171</v>
+      </c>
+      <c r="B9" s="11" t="str">
+        <f>VLOOKUP($A9,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a1d,6714d62959be40a379e53a1e,6714d62959be40a379e53a1f</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>14</v>
@@ -713,53 +940,46 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
-        <v>137</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>34</v>
+        <v>176</v>
+      </c>
+      <c r="B10" s="11" t="str">
+        <f>VLOOKUP($A10,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a29,6714d62959be40a379e53a2a,6714d62959be40a379e53a2b,6714d62959be40a379e53a2c</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
-        <v>171</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>35</v>
+        <v>229</v>
+      </c>
+      <c r="B11" s="11" t="str">
+        <f>VLOOKUP($A11,IDS!B:C,2,0)</f>
+        <v>6714d62959be40a379e53a25,6714d62959be40a379e53a26,6714d62959be40a379e53a276714d62959be40a379e53a28</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="7">
-        <v>161</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
@@ -770,15 +990,661 @@
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CE0FD75-4228-4218-A0E8-C7FACB9DF32F}">
+  <dimension ref="A1:C89"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>10</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>122</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>137</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>32</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>34</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>171</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>87</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>229</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>176</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>161</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="10"/>
+    </row>
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B26">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B29">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B36">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B46">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B56">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60" s="10"/>
+    </row>
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B61">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B62">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63" s="10"/>
+    </row>
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B66">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" s="10"/>
+    </row>
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B69">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B70">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A71" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B71">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B72">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A74" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B74">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A75" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A76" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B76">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B77">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78" s="10"/>
+    </row>
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B79">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B81">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A82" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B84">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B85">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A86" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B86">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A87" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B87">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="10"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added requirements.txt and updated eval to handle multimple embeddings
</commit_message>
<xml_diff>
--- a/backend/evaluation/FAQ.xlsx
+++ b/backend/evaluation/FAQ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danam\Git\semester_6\LAB\FinalProject\backend\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720536BD-07AB-4A2F-BE13-02049E538F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5BDA94-D457-402E-83B9-47AE5B4AB18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{16688047-19B4-47FE-ADAF-402B6B8A82DD}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">IDS!$A$60:$B$66</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>Who is eligible to transportation for treatments and examinations for dialysis patients up to 18 years of age?</t>
   </si>
@@ -108,9 +108,6 @@
   </si>
   <si>
     <t>answer</t>
-  </si>
-  <si>
-    <t>relevant_chunks_id</t>
   </si>
   <si>
     <t>6714d62959be40a379e53a30</t>
@@ -357,6 +354,15 @@
   </si>
   <si>
     <t>Is there aclinic for treatment of eating disorders in Holon?</t>
+  </si>
+  <si>
+    <t>relevant_chunks_id_emb1</t>
+  </si>
+  <si>
+    <t>relevant_chunks_id_emb2</t>
+  </si>
+  <si>
+    <t>relevant_chunks_id_emb3</t>
   </si>
 </sst>
 </file>
@@ -789,207 +795,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80926113-D334-437D-8812-60542D85F9A4}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.08984375" customWidth="1"/>
-    <col min="3" max="3" width="98" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="206.81640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="5.54296875" customWidth="1"/>
-    <col min="6" max="6" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="42.08984375" customWidth="1"/>
+    <col min="5" max="5" width="98" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="206.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="5.54296875" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>10</v>
       </c>
-      <c r="B2" s="11" t="str">
-        <f>VLOOKUP($A2,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e539ef,6714d62959be40a379e539f0,6714d62959be40a379e539f1</v>
-      </c>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="7">
         <v>32</v>
       </c>
-      <c r="B3" s="11" t="str">
-        <f>VLOOKUP($A3,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a16,6714d62959be40a379e53a17,6714d62959be40a379e53a18,6714d62959be40a379e53a19,6714d62959be40a379e53a1a</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="7">
         <v>34</v>
       </c>
-      <c r="B4" s="11" t="str">
-        <f>VLOOKUP($A4,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a1b,6714d62959be40a379e53a1c</v>
-      </c>
-      <c r="C4" s="8" t="s">
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="7">
         <v>87</v>
       </c>
-      <c r="B5" s="11" t="str">
-        <f>VLOOKUP($A5,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a20,6714d62959be40a379e53a21,6714d62959be40a379e53a22,6714d62959be40a379e53a23,6714d62959be40a379e53a24</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="7">
         <v>122</v>
       </c>
-      <c r="B6" s="11" t="str">
-        <f>VLOOKUP($A6,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e539f2,6714d62959be40a379e539f3</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="304.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="7">
         <v>137</v>
       </c>
-      <c r="B7" s="11" t="str">
-        <f>VLOOKUP($A7,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e539f4,6714d62959be40a379e539f5,6714d62959be40a379e539f6,6714d62959be40a379e539f7,6714d62959be40a379e539f8,6714d62959be40a379e539f9,6714d62959be40a379e539fa,6714d62959be40a379e539fb,6714d62959be40a379e539fc,6714d62959be40a379e539fd,6714d62959be40a379e539fe,6714d62959be40a379e539ff,6714d62959be40a379e53a00,6714d62959be40a379e53a01,6714d62959be40a379e53a02,6714d62959be40a379e53a03,6714d62959be40a379e53a04,6714d62959be40a379e53a05,6714d62959be40a379e53a06,6714d62959be40a379e53a07,6714d62959be40a379e53a08,6714d62959be40a379e53a09,6714d62959be40a379e53a0a,6714d62959be40a379e53a0b,6714d62959be40a379e53a0c,6714d62959be40a379e53a0d,6714d62959be40a379e53a0e,6714d62959be40a379e53a0f,6714d62959be40a379e53a10,6714d62959be40a379e53a11,6714d62959be40a379e53a12,6714d62959be40a379e53a13,6714d62959be40a379e53a14,6714d62959be40a379e53a15</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="F7" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="7">
         <v>161</v>
       </c>
-      <c r="B8" s="11" t="str">
-        <f>VLOOKUP($A8,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a2d,6714d62959be40a379e53a2e,6714d62959be40a379e53a2f,6714d62959be40a379e53a30</v>
-      </c>
-      <c r="C8" s="9" t="s">
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="7">
         <v>171</v>
       </c>
-      <c r="B9" s="11" t="str">
-        <f>VLOOKUP($A9,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a1d,6714d62959be40a379e53a1e,6714d62959be40a379e53a1f</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="7">
         <v>176</v>
       </c>
-      <c r="B10" s="11" t="str">
-        <f>VLOOKUP($A10,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a29,6714d62959be40a379e53a2a,6714d62959be40a379e53a2b,6714d62959be40a379e53a2c</v>
-      </c>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="7">
         <v>229</v>
       </c>
-      <c r="B11" s="11" t="str">
-        <f>VLOOKUP($A11,IDS!B:C,2,0)</f>
-        <v>6714d62959be40a379e53a25,6714d62959be40a379e53a26,6714d62959be40a379e53a276714d62959be40a379e53a28</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1018,7 +1028,7 @@
         <v>10</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -1026,7 +1036,7 @@
         <v>122</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -1034,7 +1044,7 @@
         <v>137</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -1042,7 +1052,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -1050,7 +1060,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -1058,7 +1068,7 @@
         <v>171</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -1066,7 +1076,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -1074,7 +1084,7 @@
         <v>229</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -1082,7 +1092,7 @@
         <v>176</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -1090,7 +1100,7 @@
         <v>161</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -1098,7 +1108,7 @@
     </row>
     <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13">
         <v>10</v>
@@ -1106,7 +1116,7 @@
     </row>
     <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B14">
         <v>10</v>
@@ -1114,7 +1124,7 @@
     </row>
     <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -1123,7 +1133,7 @@
     <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
     <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17">
         <v>122</v>
@@ -1131,7 +1141,7 @@
     </row>
     <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18">
         <v>122</v>
@@ -1139,7 +1149,7 @@
     </row>
     <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20">
         <v>137</v>
@@ -1147,7 +1157,7 @@
     </row>
     <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21">
         <v>137</v>
@@ -1155,7 +1165,7 @@
     </row>
     <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>137</v>
@@ -1163,7 +1173,7 @@
     </row>
     <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>137</v>
@@ -1171,7 +1181,7 @@
     </row>
     <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24">
         <v>137</v>
@@ -1179,7 +1189,7 @@
     </row>
     <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B25">
         <v>137</v>
@@ -1187,7 +1197,7 @@
     </row>
     <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B26">
         <v>137</v>
@@ -1195,7 +1205,7 @@
     </row>
     <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27">
         <v>137</v>
@@ -1203,7 +1213,7 @@
     </row>
     <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B28">
         <v>137</v>
@@ -1211,7 +1221,7 @@
     </row>
     <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B29">
         <v>137</v>
@@ -1219,7 +1229,7 @@
     </row>
     <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B30">
         <v>137</v>
@@ -1227,7 +1237,7 @@
     </row>
     <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B31">
         <v>137</v>
@@ -1235,7 +1245,7 @@
     </row>
     <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B32">
         <v>137</v>
@@ -1243,7 +1253,7 @@
     </row>
     <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33">
         <v>137</v>
@@ -1251,7 +1261,7 @@
     </row>
     <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B34">
         <v>137</v>
@@ -1259,7 +1269,7 @@
     </row>
     <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B35">
         <v>137</v>
@@ -1267,7 +1277,7 @@
     </row>
     <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36">
         <v>137</v>
@@ -1275,7 +1285,7 @@
     </row>
     <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B37">
         <v>137</v>
@@ -1283,7 +1293,7 @@
     </row>
     <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B38">
         <v>137</v>
@@ -1291,7 +1301,7 @@
     </row>
     <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B39">
         <v>137</v>
@@ -1299,7 +1309,7 @@
     </row>
     <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B40">
         <v>137</v>
@@ -1307,7 +1317,7 @@
     </row>
     <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B41">
         <v>137</v>
@@ -1315,7 +1325,7 @@
     </row>
     <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42">
         <v>137</v>
@@ -1323,7 +1333,7 @@
     </row>
     <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43">
         <v>137</v>
@@ -1331,7 +1341,7 @@
     </row>
     <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44">
         <v>137</v>
@@ -1339,7 +1349,7 @@
     </row>
     <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45">
         <v>137</v>
@@ -1347,7 +1357,7 @@
     </row>
     <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B46">
         <v>137</v>
@@ -1355,7 +1365,7 @@
     </row>
     <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B47">
         <v>137</v>
@@ -1363,7 +1373,7 @@
     </row>
     <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B48">
         <v>137</v>
@@ -1371,7 +1381,7 @@
     </row>
     <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B49">
         <v>137</v>
@@ -1379,7 +1389,7 @@
     </row>
     <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B50">
         <v>137</v>
@@ -1387,7 +1397,7 @@
     </row>
     <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B51">
         <v>137</v>
@@ -1395,7 +1405,7 @@
     </row>
     <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B52">
         <v>137</v>
@@ -1403,7 +1413,7 @@
     </row>
     <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B53">
         <v>137</v>
@@ -1411,7 +1421,7 @@
     </row>
     <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55">
         <v>32</v>
@@ -1419,7 +1429,7 @@
     </row>
     <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B56">
         <v>32</v>
@@ -1427,7 +1437,7 @@
     </row>
     <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57">
         <v>32</v>
@@ -1435,7 +1445,7 @@
     </row>
     <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B58">
         <v>32</v>
@@ -1443,7 +1453,7 @@
     </row>
     <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59">
         <v>32</v>
@@ -1454,7 +1464,7 @@
     </row>
     <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B61">
         <v>34</v>
@@ -1462,7 +1472,7 @@
     </row>
     <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B62">
         <v>34</v>
@@ -1473,7 +1483,7 @@
     </row>
     <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B64">
         <v>171</v>
@@ -1481,7 +1491,7 @@
     </row>
     <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B65">
         <v>171</v>
@@ -1489,7 +1499,7 @@
     </row>
     <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B66">
         <v>171</v>
@@ -1500,7 +1510,7 @@
     </row>
     <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B68">
         <v>87</v>
@@ -1508,7 +1518,7 @@
     </row>
     <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B69">
         <v>87</v>
@@ -1516,7 +1526,7 @@
     </row>
     <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B70">
         <v>87</v>
@@ -1524,7 +1534,7 @@
     </row>
     <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B71">
         <v>87</v>
@@ -1532,7 +1542,7 @@
     </row>
     <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B72">
         <v>87</v>
@@ -1540,7 +1550,7 @@
     </row>
     <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B74">
         <v>229</v>
@@ -1548,7 +1558,7 @@
     </row>
     <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B75">
         <v>229</v>
@@ -1556,7 +1566,7 @@
     </row>
     <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B76">
         <v>229</v>
@@ -1564,7 +1574,7 @@
     </row>
     <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B77">
         <v>229</v>
@@ -1575,7 +1585,7 @@
     </row>
     <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B79">
         <v>176</v>
@@ -1583,7 +1593,7 @@
     </row>
     <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B80">
         <v>176</v>
@@ -1591,7 +1601,7 @@
     </row>
     <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B81">
         <v>176</v>
@@ -1599,7 +1609,7 @@
     </row>
     <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B82">
         <v>176</v>
@@ -1607,7 +1617,7 @@
     </row>
     <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B84">
         <v>161</v>
@@ -1615,7 +1625,7 @@
     </row>
     <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B85">
         <v>161</v>
@@ -1623,7 +1633,7 @@
     </row>
     <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86">
         <v>161</v>
@@ -1631,7 +1641,7 @@
     </row>
     <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B87">
         <v>161</v>

</xml_diff>

<commit_message>
added origin file to chunks, changed Cohere API key
</commit_message>
<xml_diff>
--- a/backend/evaluation/FAQ.xlsx
+++ b/backend/evaluation/FAQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danam\Git\semester_6\LAB\FinalProject\backend\evaluation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Saar/PycharmProjects/FinalProject/backend/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5BDA94-D457-402E-83B9-47AE5B4AB18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CDB79E-6B3A-1942-946F-D9DA8AFE0E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{16688047-19B4-47FE-ADAF-402B6B8A82DD}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="19440" xr2:uid="{16688047-19B4-47FE-ADAF-402B6B8A82DD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,13 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
-  <si>
-    <t>Who is eligible to transportation for treatments and examinations for dialysis patients up to 18 years of age?</t>
-  </si>
-  <si>
-    <t>How much Examination and treatment for vision focus cost?</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="131">
   <si>
     <t>Children and youth members of the Maccabi are dialysis patients who are not yet 18 years old, traveling for treatment in a hospital, at a dedicated dialysis institute for children. Eligibility for dialysis patients under the age of 18</t>
   </si>
@@ -64,9 +58,6 @@
     <t xml:space="preserve">At Maccabi Mental Health Clinics. </t>
   </si>
   <si>
-    <t>Does doctor's referral is necessary to do a test in order toidentify my blood type?</t>
-  </si>
-  <si>
     <t>A doctor's referral is necessary.</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
   </si>
   <si>
     <t>Visit to a specialist - 36₪ quarterly deductible</t>
-  </si>
-  <si>
-    <t>doc_id</t>
   </si>
   <si>
     <t>question</t>
@@ -363,6 +351,105 @@
   </si>
   <si>
     <t>relevant_chunks_id_emb3</t>
+  </si>
+  <si>
+    <t>Is a doctor's referral necessary to do a test to determine my blood type?</t>
+  </si>
+  <si>
+    <t>Who is eligible for transportation for treatments and examinations for dialysis patients up to 18 years of age?</t>
+  </si>
+  <si>
+    <t>671abd8cc063150696ff9517</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf2088b</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208a4,671b904d95b27ff0ddf208a5,671b904d95b27ff0ddf208a6,671b904d95b27ff0ddf208a7,671b904d95b27ff0ddf208a8,671b904d95b27ff0ddf208a9,671b904d95b27ff0ddf208aa,671b904d95b27ff0ddf208ab,671b904d95b27ff0ddf208ac,671b904d95b27ff0ddf208ad,671b904d95b27ff0ddf208ae,671b904d95b27ff0ddf208af,671b904d95b27ff0ddf208b0,671b904d95b27ff0ddf208b1,671b904d95b27ff0ddf208b2,671b904d95b27ff0ddf208b3,671b904d95b27ff0ddf208b4,671b904d95b27ff0ddf208b5,671b904d95b27ff0ddf208b6,671b904d95b27ff0ddf208b7,671b904d95b27ff0ddf208b8,671b904d95b27ff0ddf208b9</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208e4,671b904d95b27ff0ddf208e5</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208fd,671b904d95b27ff0ddf208fe,671b904d95b27ff0ddf208dc,671b904d95b27ff0ddf208dd,671b904d95b27ff0ddf20889,671b904d95b27ff0ddf2088a</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208f8,671b904d95b27ff0ddf208f9</t>
+  </si>
+  <si>
+    <t>How much do examination and treatment for vision focus cost?</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208f1</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208ea,671b904d95b27ff0ddf208eb,671b904d95b27ff0ddf208ec</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208d7</t>
+  </si>
+  <si>
+    <t>671b904d95b27ff0ddf208bb,671b904d95b27ff0ddf208bc</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf2098c,671b909b95b27ff0ddf2098d</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf2095c</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209a8</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209bb,671b909b95b27ff0ddf209bc,671b909b95b27ff0ddf209bd</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf20971</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf20975,671b909b95b27ff0ddf20976,671b909b95b27ff0ddf20977,671b909b95b27ff0ddf20978,671b909b95b27ff0ddf20979,671b909b95b27ff0ddf2097a,671b909b95b27ff0ddf2097b,671b909b95b27ff0ddf2097c,671b909b95b27ff0ddf2097d,671b909b95b27ff0ddf2097e,671b909b95b27ff0ddf2097f,671b909b95b27ff0ddf20980,671b909b95b27ff0ddf20981,671b909b95b27ff0ddf20982,671b909b95b27ff0ddf20983,671b909b95b27ff0ddf20984,671b909b95b27ff0ddf20985,671b909b95b27ff0ddf20986,671b909b95b27ff0ddf20987,671b909b95b27ff0ddf20988,671b909b95b27ff0ddf20989,671b909b95b27ff0ddf2098a</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209ce,671b909b95b27ff0ddf209cf</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209b5,671b909b95b27ff0ddf209b6</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209c9,671b909b95b27ff0ddf209ca</t>
+  </si>
+  <si>
+    <t>671b909b95b27ff0ddf209c2</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a93</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a9a,671b90a595b27ff0ddf20a9b</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a86,671b90a595b27ff0ddf20a87</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a9f,671b90a595b27ff0ddf20aa0</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a2d</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a5d,671b90a595b27ff0ddf20a5e</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a79</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a8c,671b90a595b27ff0ddf20a8d,671b90a595b27ff0ddf20a8e</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a42</t>
+  </si>
+  <si>
+    <t>671b90a595b27ff0ddf20a46,671b90a595b27ff0ddf20a47,671b90a595b27ff0ddf20a48,671b90a595b27ff0ddf20a49,671b90a595b27ff0ddf20a4a,671b90a595b27ff0ddf20a4b,671b90a595b27ff0ddf20a4c,671b90a595b27ff0ddf20a4d,671b90a595b27ff0ddf20a4e,671b90a595b27ff0ddf20a4f,671b90a595b27ff0ddf20a50,671b90a595b27ff0ddf20a51,671b90a595b27ff0ddf20a52,671b90a595b27ff0ddf20a53,671b90a595b27ff0ddf20a54,671b90a595b27ff0ddf20a55,671b90a595b27ff0ddf20a56,671b90a595b27ff0ddf20a57,671b90a595b27ff0ddf20a58,671b90a595b27ff0ddf20a59,671b90a595b27ff0ddf20a5a,671b90a595b27ff0ddf20a5b</t>
   </si>
 </sst>
 </file>
@@ -797,182 +884,244 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80926113-D334-437D-8812-60542D85F9A4}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="42.08984375" customWidth="1"/>
-    <col min="5" max="5" width="98" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="206.81640625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="5.54296875" customWidth="1"/>
-    <col min="8" max="8" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="81" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="60" style="2" customWidth="1"/>
+    <col min="7" max="7" width="54.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>126</v>
       </c>
       <c r="B1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="7">
         <v>10</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
+      <c r="B2" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>125</v>
+      </c>
       <c r="E2" s="8" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" s="7">
         <v>32</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="B3" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>126</v>
+      </c>
       <c r="E3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>34</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+      <c r="B4" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="E4" s="8" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="7">
         <v>87</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
+      <c r="B5" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>128</v>
+      </c>
       <c r="E5" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:6" ht="38" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>122</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D6" t="s">
+        <v>129</v>
+      </c>
       <c r="E6" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7">
         <v>137</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
+      <c r="B7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" t="s">
+        <v>130</v>
+      </c>
       <c r="E7" s="8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="58" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>161</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
+      <c r="B8" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>124</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="7">
         <v>171</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="E9" s="8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>176</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
+      <c r="B10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>122</v>
+      </c>
       <c r="E10" s="8" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="7">
         <v>229</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
+      <c r="B11" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="E11" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -980,21 +1129,21 @@
       <c r="E12" s="1"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1016,641 +1165,641 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="61.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>10</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>122</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B3">
         <v>137</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>32</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B5">
         <v>34</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B6">
         <v>171</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B7">
         <v>87</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>229</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B9">
         <v>176</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B10">
         <v>161</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="C11" s="10"/>
     </row>
-    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B13">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B15">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B18">
         <v>122</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B20">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="10" t="s">
+      <c r="B23">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="B21">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="B26">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B22">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="10" t="s">
+      <c r="B27">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B23">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="10" t="s">
+      <c r="B28">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B24">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="10" t="s">
+      <c r="B29">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B26">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="10" t="s">
+      <c r="B30">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B27">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="10" t="s">
+      <c r="B31">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="B28">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="10" t="s">
+      <c r="B32">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="B29">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="10" t="s">
+      <c r="B33">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B30">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="10" t="s">
+      <c r="B34">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B31">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="10" t="s">
+      <c r="B35">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B32">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="10" t="s">
+      <c r="B36">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="B33">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="10" t="s">
+      <c r="B37">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B34">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="10" t="s">
+      <c r="B38">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B35">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="10" t="s">
+      <c r="B39">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B36">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="10" t="s">
+      <c r="B40">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B37">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="10" t="s">
+      <c r="B41">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B38">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="10" t="s">
+      <c r="B42">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B46">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B47">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="B39">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="10" t="s">
+      <c r="B48">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B40">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="10" t="s">
+      <c r="B49">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="B41">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="10" t="s">
+      <c r="B50">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B42">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B43">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="B44">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="B45">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B47">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="10" t="s">
+      <c r="B51">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B48">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="10" t="s">
+      <c r="B52">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B49">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B50">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="B53">
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B55">
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B56">
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B57">
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="10" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B58">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B59">
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="10"/>
     </row>
-    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="10" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B61">
         <v>34</v>
       </c>
     </row>
-    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B62">
         <v>34</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="10"/>
     </row>
-    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B64">
         <v>171</v>
       </c>
     </row>
-    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B65">
         <v>171</v>
       </c>
     </row>
-    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="10" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B66">
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="10"/>
     </row>
-    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="10" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B68">
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B69">
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B70">
         <v>87</v>
       </c>
     </row>
-    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B71">
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B72">
         <v>87</v>
       </c>
     </row>
-    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="10" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B74">
         <v>229</v>
       </c>
     </row>
-    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B75">
         <v>229</v>
       </c>
     </row>
-    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="10" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B76">
         <v>229</v>
       </c>
     </row>
-    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="10" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B77">
         <v>229</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="10"/>
     </row>
-    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B79">
         <v>176</v>
       </c>
     </row>
-    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B80">
         <v>176</v>
       </c>
     </row>
-    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B81">
         <v>176</v>
       </c>
     </row>
-    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="10" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B82">
         <v>176</v>
       </c>
     </row>
-    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="10" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B84">
         <v>161</v>
       </c>
     </row>
-    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B85">
         <v>161</v>
       </c>
     </row>
-    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B86">
         <v>161</v>
       </c>
     </row>
-    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:2" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B87">
         <v>161</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="10"/>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="10"/>
     </row>
   </sheetData>

</xml_diff>